<commit_message>
Fulfill 36 scientific names in typo_vlookup
</commit_message>
<xml_diff>
--- a/input_xlsx/Hassan 001.xlsx
+++ b/input_xlsx/Hassan 001.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Biodiverskripsi\Papua\Skripsi &amp; Transkripsi\Hassan\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6A3804-615E-4DF6-A550-099D6518919B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19420" windowHeight="11020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Events" sheetId="2" r:id="rId1"/>
@@ -18,7 +12,7 @@
     <sheet name="Literature" sheetId="6" r:id="rId3"/>
     <sheet name="Measurement" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,13 +27,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Kyle Braak</author>
     <author>Primadieta</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CD98E0A5-3498-464D-8C1F-A0E35C7CE151}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{B62A1221-E2EF-4626-A002-493B3C61FEF9}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -303,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3F3BB270-74F1-4DCB-B8B5-71EBB6C85A4C}">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -347,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -391,7 +385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -435,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -479,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -523,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -611,7 +605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -655,7 +649,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -699,7 +693,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000010000000}">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -743,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000011000000}">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -787,7 +781,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000012000000}">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -831,7 +825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{296C6269-92AD-4202-BA90-ADA4FA29AB61}">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -875,7 +869,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{3ED38722-4F9B-4031-863A-CC37137E1DB2}">
+    <comment ref="T1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -904,13 +898,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Kyle Braak</author>
     <author>Primadieta</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -954,7 +948,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -998,7 +992,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1042,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1086,7 +1080,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1130,7 +1124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1184,7 +1178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1228,7 +1222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{CBD564F0-F558-411F-9EA6-B347A9C3AF66}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1272,7 +1266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1316,7 +1310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1360,7 +1354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1448,7 +1442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1492,7 +1486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1580,7 +1574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1624,7 +1618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{94D49537-4BE7-4234-BC89-0F660595960E}">
+    <comment ref="Q1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1653,13 +1647,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Kyle Braak</author>
     <author>Primadieta</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{36AAAF2B-60DB-4D04-A886-FCFB68D4557C}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1703,7 +1697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5855233F-3735-4892-B9ED-9E8A494DD76A}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1747,7 +1741,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{654440DE-876B-46A0-AD15-F6A1DB049347}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1791,7 +1785,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{9C17C331-E974-4CC2-87EF-BF0DE1E2FBE1}">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1835,7 +1829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{A2A38E94-5E62-46F5-BF6D-82257421DB5D}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1879,7 +1873,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{7DD737BE-C816-4739-81DA-E2164ADBEC35}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1923,7 +1917,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{397DE40C-8F94-4168-B2C9-39AE2BDEAD84}">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1967,7 +1961,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{82624C0C-C579-47F5-B3CC-8570BE7C1321}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2011,7 +2005,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{C7C77C63-8193-4F82-AEC0-0727572A49AD}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2055,7 +2049,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{E14C9CF2-28E1-4DAE-932B-A79FD12BBA60}">
+    <comment ref="J1" authorId="1">
       <text>
         <r>
           <rPr>
@@ -2084,12 +2078,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Kyle Braak</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A9AD44FF-D45C-4CF7-8D68-1F16CECDC920}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2133,7 +2127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2177,7 +2171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EA51D073-7D69-4871-BBDD-42ACFD92F7EF}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2202,7 +2196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{2281CE55-2B75-44E9-B998-E323939D1033}">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2246,7 +2240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{30A37606-FB54-415C-BC94-2ADDE96B908F}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2290,7 +2284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{F05604D2-DAE8-4B31-BC64-2DB4383D2D2A}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2334,7 +2328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{4D4B6592-D3BE-48AA-887F-614FC81C00AA}">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2378,7 +2372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{D4DD68B5-C1F0-406C-89E1-176B6CFEE35A}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2422,7 +2416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{D52C51D3-943B-4902-B5FE-D5D765B0EAB6}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2471,7 +2465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="178">
   <si>
     <t>occurrenceID</t>
   </si>
@@ -3628,11 +3622,32 @@
   <si>
     <t>Musa</t>
   </si>
+  <si>
+    <t>UNCEN-2000NL-HS001-PM001-VE001</t>
+  </si>
+  <si>
+    <t>UNCEN-2000NL-HS001-PM001-VE002</t>
+  </si>
+  <si>
+    <t>UNCEN-2000NL-HS001-PM001-VE003</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Phalanger orientalis</t>
+  </si>
+  <si>
+    <t>Phalanger permixtio</t>
+  </si>
+  <si>
+    <t>Spilocuscus maculatus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4365,15 +4380,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.25" bestFit="1" customWidth="1"/>
@@ -4381,19 +4396,19 @@
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.08203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="10" width="14.875" customWidth="1"/>
-    <col min="11" max="11" width="17.625" customWidth="1"/>
+    <col min="9" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="17.58203125" customWidth="1"/>
     <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="16.125" customWidth="1"/>
+    <col min="13" max="13" width="16.08203125" customWidth="1"/>
     <col min="14" max="17" width="13.5" customWidth="1"/>
     <col min="18" max="18" width="13.25" customWidth="1"/>
     <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="54.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -4455,7 +4470,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -4514,16 +4529,16 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E3"/>
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="K4" s="11"/>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E5" s="9"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
@@ -4542,35 +4557,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="M15" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33:P36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.58203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="15.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.875" customWidth="1"/>
-    <col min="10" max="10" width="18.625" customWidth="1"/>
-    <col min="11" max="11" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="15.08203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18.58203125" customWidth="1"/>
+    <col min="11" max="11" width="15.58203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.58203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.75" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="157.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -4623,7 +4638,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -4667,7 +4682,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -4711,7 +4726,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4755,7 +4770,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -4799,7 +4814,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4843,7 +4858,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4887,7 +4902,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -4931,7 +4946,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -4975,7 +4990,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -5019,7 +5034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -5063,7 +5078,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -5107,7 +5122,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -5151,7 +5166,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -5195,7 +5210,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -5239,7 +5254,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -5283,7 +5298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -5327,7 +5342,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -5371,7 +5386,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -5415,7 +5430,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -5459,7 +5474,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -5503,7 +5518,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -5547,7 +5562,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -5591,7 +5606,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -5635,7 +5650,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -5679,7 +5694,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -5723,7 +5738,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -5767,7 +5782,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -5811,7 +5826,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -5855,7 +5870,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -5899,7 +5914,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -5943,7 +5958,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -5987,7 +6002,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -6029,6 +6044,129 @@
       </c>
       <c r="Q33" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" t="s">
+        <v>106</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" t="s">
+        <v>48</v>
+      </c>
+      <c r="M34" t="s">
+        <v>65</v>
+      </c>
+      <c r="P34" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K35" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" t="s">
+        <v>48</v>
+      </c>
+      <c r="M35" t="s">
+        <v>65</v>
+      </c>
+      <c r="P35" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" t="s">
+        <v>48</v>
+      </c>
+      <c r="M36" t="s">
+        <v>65</v>
+      </c>
+      <c r="P36" s="17" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -6045,7 +6183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
@@ -6053,21 +6191,21 @@
       <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="17.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="34.5" customWidth="1"/>
     <col min="9" max="9" width="19.25" customWidth="1"/>
-    <col min="10" max="10" width="39.375" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -6099,7 +6237,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -6136,27 +6274,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.75" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="21.75" customWidth="1"/>
     <col min="7" max="7" width="19.75" customWidth="1"/>
-    <col min="8" max="8" width="28.625" customWidth="1"/>
-    <col min="9" max="9" width="22.625" customWidth="1"/>
+    <col min="8" max="8" width="28.58203125" customWidth="1"/>
+    <col min="9" max="9" width="22.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>